<commit_message>
modifier code arduino fix some bug for new matome insert machine
</commit_message>
<xml_diff>
--- a/FORM PROGRAM MATOME_LED _TABLE.xlsx
+++ b/FORM PROGRAM MATOME_LED _TABLE.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -683,13 +683,13 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,7 +1244,7 @@
       <c r="M18" s="2">
         <v>8</v>
       </c>
-      <c r="N18" s="35" t="s">
+      <c r="N18" s="36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
         <f>M18+8</f>
         <v>16</v>
       </c>
-      <c r="N19" s="35"/>
+      <c r="N19" s="36"/>
     </row>
     <row r="20" spans="11:14">
       <c r="K20" s="11" t="s">
@@ -1264,49 +1264,49 @@
         <f t="shared" ref="M20:M33" si="0">M19+8</f>
         <v>24</v>
       </c>
-      <c r="N20" s="35"/>
+      <c r="N20" s="36"/>
     </row>
     <row r="21" spans="11:14">
       <c r="M21" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="N21" s="35"/>
+      <c r="N21" s="36"/>
     </row>
     <row r="22" spans="11:14">
       <c r="M22" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="N22" s="35"/>
+      <c r="N22" s="36"/>
     </row>
     <row r="23" spans="11:14">
       <c r="M23" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="N23" s="35"/>
+      <c r="N23" s="36"/>
     </row>
     <row r="24" spans="11:14">
       <c r="M24" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="N24" s="35"/>
+      <c r="N24" s="36"/>
     </row>
     <row r="25" spans="11:14">
       <c r="M25" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="N25" s="35"/>
+      <c r="N25" s="36"/>
     </row>
     <row r="26" spans="11:14">
       <c r="M26" s="2">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="N26" s="35" t="s">
+      <c r="N26" s="36" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1315,49 +1315,49 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="N27" s="35"/>
+      <c r="N27" s="36"/>
     </row>
     <row r="28" spans="11:14">
       <c r="M28" s="2">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="N28" s="35"/>
+      <c r="N28" s="36"/>
     </row>
     <row r="29" spans="11:14">
       <c r="M29" s="2">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="N29" s="35"/>
+      <c r="N29" s="36"/>
     </row>
     <row r="30" spans="11:14">
       <c r="M30" s="2">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="N30" s="35"/>
+      <c r="N30" s="36"/>
     </row>
     <row r="31" spans="11:14">
       <c r="M31" s="2">
         <f>M30+8</f>
         <v>112</v>
       </c>
-      <c r="N31" s="35"/>
+      <c r="N31" s="36"/>
     </row>
     <row r="32" spans="11:14">
       <c r="M32" s="2">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="N32" s="35"/>
+      <c r="N32" s="36"/>
     </row>
     <row r="33" spans="11:14">
       <c r="M33" s="2">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="N33" s="35"/>
+      <c r="N33" s="36"/>
     </row>
     <row r="34" spans="11:14">
       <c r="K34" s="1" t="s">
@@ -1382,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BX69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AO26" sqref="AO26"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BN38" sqref="BN38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="16.5" customHeight="1"/>
@@ -3313,14 +3313,14 @@
       <c r="N21" s="23">
         <v>192</v>
       </c>
-      <c r="T21" s="36" t="s">
+      <c r="T21" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="37"/>
       <c r="Z21" s="33"/>
       <c r="AA21" s="33"/>
       <c r="AB21" s="34" t="s">
@@ -3408,19 +3408,19 @@
       <c r="Z22" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="AI22" s="37" t="s">
+      <c r="AI22" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="AJ22" s="37"/>
-      <c r="AK22" s="37"/>
-      <c r="AL22" s="37"/>
-      <c r="AM22" s="37"/>
-      <c r="AN22" s="37"/>
-      <c r="AO22" s="37"/>
-      <c r="AP22" s="37"/>
-      <c r="AQ22" s="37"/>
-      <c r="AR22" s="37"/>
-      <c r="AS22" s="37"/>
+      <c r="AJ22" s="35"/>
+      <c r="AK22" s="35"/>
+      <c r="AL22" s="35"/>
+      <c r="AM22" s="35"/>
+      <c r="AN22" s="35"/>
+      <c r="AO22" s="35"/>
+      <c r="AP22" s="35"/>
+      <c r="AQ22" s="35"/>
+      <c r="AR22" s="35"/>
+      <c r="AS22" s="35"/>
       <c r="BA22" s="12" t="s">
         <v>79</v>
       </c>

</xml_diff>